<commit_message>
add convert and add mapping muti cell one pojo
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,38 @@
   </si>
   <si>
     <t>jiji2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>细菌名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>药1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>药2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耐药</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛逼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -389,18 +421,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,8 +446,23 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -427,8 +475,20 @@
       <c r="D2" s="2">
         <v>23</v>
       </c>
+      <c r="E2" s="1">
+        <v>41996</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
add position in inspect info
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,14 @@
   </si>
   <si>
     <t>牛逼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胸部</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -421,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -433,7 +441,7 @@
     <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,8 +469,11 @@
       <c r="I1" t="s">
         <v>10</v>
       </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -487,8 +498,11 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
move distinct method to patientgenerator and fix not add inspect bug
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,51 +42,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>jiji2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检验类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>细菌名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>药1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>药2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耐药</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛逼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胸部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>jiji</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jiji2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>检验时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>检验类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>细菌名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>药1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>药2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>耐药</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3,4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>牛逼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>部位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>胸部</t>
+  </si>
+  <si>
+    <t>jiji</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛逼2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸡巴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -455,27 +466,27 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3">
         <v>33</v>
@@ -490,21 +501,50 @@
         <v>41996</v>
       </c>
       <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42758</v>
+      </c>
+      <c r="D4" s="2">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42361</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify drupfast logic and finish report logic
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tangjijun\IdeaProjects\analyze\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,6 +101,13 @@
   </si>
   <si>
     <t>牛逼3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z495256</t>
+  </si>
+  <si>
+    <t>z495257</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -440,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -451,16 +453,16 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,12 +494,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3">
-        <v>33</v>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="1">
         <v>42727</v>
@@ -521,17 +523,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3">
-        <v>33</v>
+      <c r="B4" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>42758</v>
@@ -555,12 +557,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
-        <v>34</v>
+      <c r="B5" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="1">
         <v>42970</v>

</xml_diff>